<commit_message>
Update Pintle Calcs 12-19-19.xlsx
</commit_message>
<xml_diff>
--- a/6kN Heat Sink Engine/Pintle Calcs 12-19-19.xlsx
+++ b/6kN Heat Sink Engine/Pintle Calcs 12-19-19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcb\Documents\GitHub\liquid-propellant-engine\6kN Heat Sink Engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AB7276F-E0E5-4865-A1A6-8CE17AF78F2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77754644-C725-44D7-B182-F67B10F81D4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="2946" windowWidth="19548" windowHeight="9570" xr2:uid="{A9D4EDED-FB2F-42A7-8C07-9670575B9D2C}"/>
+    <workbookView xWindow="960" yWindow="-96" windowWidth="22176" windowHeight="13152" xr2:uid="{A9D4EDED-FB2F-42A7-8C07-9670575B9D2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Pintle Calculator</t>
   </si>
@@ -55,6 +57,15 @@
   </si>
   <si>
     <t>Pintle Gap</t>
+  </si>
+  <si>
+    <t>Momentum ratio</t>
+  </si>
+  <si>
+    <t>LOX velocity</t>
+  </si>
+  <si>
+    <t>m/s</t>
   </si>
 </sst>
 </file>
@@ -114,6 +125,116 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>118110</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>567690</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D6D9585-D56C-4D63-8505-D1C59D694244}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2190750" y="2282190"/>
+          <a:ext cx="1059180" cy="601980"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>575310</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>72611</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83B7E735-F78D-4A3C-962C-848381570BDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3383280" y="2190750"/>
+          <a:ext cx="1703070" cy="807941"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,74 +534,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2410FA10-B613-474A-BEF8-4DDACA0CA65C}">
-  <dimension ref="A3:C11"/>
+  <dimension ref="A3:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.47265625" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1">
-        <f>0.8*25.4</f>
-        <v>20.32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+      <c r="C9" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="1">
-        <f>2*(B11/3.1415+(C6/2)^2)^0.5</f>
-        <v>23.333065038967447</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+      <c r="C10" s="1">
+        <f>2*(B14/3.1415+(C9/2)^2)^0.5</f>
+        <v>29.334783519103819</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
-        <f>130/(PI()*C6)</f>
-        <v>2.0364313584592906</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+      <c r="C11" s="1">
+        <f>B13/(PI()*C9)</f>
+        <v>1.532603155699733</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B10">
+      <c r="B13">
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B11">
+      <c r="B14">
         <v>103.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>